<commit_message>
Updated Arclight matchups, added counter score to tier display
</commit_message>
<xml_diff>
--- a/Mechabellum Unit Counters.xlsx
+++ b/Mechabellum Unit Counters.xlsx
@@ -164,7 +164,7 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -383,12 +383,10 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="13.0"/>
-    <col customWidth="1" min="2" max="2" width="7.13"/>
-    <col customWidth="1" min="3" max="3" width="5.0"/>
-    <col customWidth="1" min="4" max="4" width="6.25"/>
+    <col customWidth="1" min="2" max="4" width="7.13"/>
     <col customWidth="1" min="5" max="5" width="9.25"/>
     <col customWidth="1" min="6" max="6" width="7.25"/>
-    <col customWidth="1" min="7" max="7" width="5.38"/>
+    <col customWidth="1" min="7" max="7" width="7.13"/>
     <col customWidth="1" min="8" max="8" width="7.88"/>
     <col customWidth="1" min="9" max="9" width="13.0"/>
     <col customWidth="1" min="10" max="10" width="8.5"/>
@@ -397,21 +395,18 @@
     <col customWidth="1" min="13" max="13" width="11.63"/>
     <col customWidth="1" min="14" max="14" width="8.38"/>
     <col customWidth="1" min="15" max="15" width="9.75"/>
-    <col customWidth="1" min="16" max="16" width="5.75"/>
-    <col customWidth="1" min="17" max="17" width="6.5"/>
-    <col customWidth="1" min="18" max="18" width="6.13"/>
+    <col customWidth="1" min="16" max="18" width="7.13"/>
     <col customWidth="1" min="19" max="19" width="8.25"/>
-    <col customWidth="1" min="20" max="20" width="6.38"/>
+    <col customWidth="1" min="20" max="20" width="7.13"/>
     <col customWidth="1" min="21" max="21" width="7.63"/>
     <col customWidth="1" min="22" max="22" width="11.5"/>
     <col customWidth="1" min="23" max="23" width="9.5"/>
-    <col customWidth="1" min="24" max="24" width="6.5"/>
+    <col customWidth="1" min="24" max="24" width="7.13"/>
     <col customWidth="1" min="25" max="25" width="8.0"/>
     <col customWidth="1" min="26" max="26" width="10.63"/>
     <col customWidth="1" min="27" max="27" width="10.25"/>
     <col customWidth="1" min="28" max="28" width="7.88"/>
-    <col customWidth="1" min="29" max="29" width="7.0"/>
-    <col customWidth="1" min="30" max="30" width="6.0"/>
+    <col customWidth="1" min="29" max="30" width="7.13"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -896,7 +891,7 @@
         <v>33</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>31</v>
@@ -917,19 +912,19 @@
         <v>31</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>33</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="T6" s="3" t="s">
         <v>31</v>
@@ -953,7 +948,7 @@
         <v>33</v>
       </c>
       <c r="AA6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB6" s="3" t="s">
         <v>31</v>
@@ -1074,7 +1069,7 @@
         <v>30</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>30</v>
@@ -1718,7 +1713,7 @@
         <v>29</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>33</v>
@@ -1810,7 +1805,7 @@
         <v>29</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>33</v>
@@ -1902,7 +1897,7 @@
         <v>33</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>33</v>
@@ -2822,7 +2817,7 @@
         <v>31</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>33</v>
@@ -2914,7 +2909,7 @@
         <v>31</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>34</v>
@@ -3384,6 +3379,11 @@
       <c r="A100" s="1"/>
     </row>
   </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B2:AD30">
+      <formula1>"S,A,B,C,D,F"</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>